<commit_message>
Màj du Word avec début explication code
</commit_message>
<xml_diff>
--- a/Data_test.xlsx
+++ b/Data_test.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S689"/>
+  <dimension ref="A1:S603"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19718,2763 +19718,11 @@
       <c r="G603" t="n">
         <v>1435.599103898377</v>
       </c>
-      <c r="I603" t="n">
-        <v>428.802201720373</v>
-      </c>
-      <c r="K603" t="n">
-        <v>-972.4781362518797</v>
-      </c>
-      <c r="M603" t="n">
-        <v>988.5534834229475</v>
-      </c>
-      <c r="O603" t="n">
-        <v>372.1991720144615</v>
-      </c>
       <c r="Q603" t="n">
         <v>1434.836771468303</v>
       </c>
       <c r="S603" t="n">
         <v>1499.618328758515</v>
-      </c>
-    </row>
-    <row r="604">
-      <c r="A604" t="n">
-        <v>1045.735454467328</v>
-      </c>
-      <c r="C604" t="n">
-        <v>663.916608758421</v>
-      </c>
-      <c r="E604" t="n">
-        <v>1647.728072802673</v>
-      </c>
-      <c r="G604" t="n">
-        <v>1435.971303070391</v>
-      </c>
-      <c r="I604" t="n">
-        <v>429.5717776053607</v>
-      </c>
-      <c r="K604" t="n">
-        <v>-972.3932021621522</v>
-      </c>
-      <c r="M604" t="n">
-        <v>988.5605853498873</v>
-      </c>
-      <c r="O604" t="n">
-        <v>372.803824605171</v>
-      </c>
-      <c r="Q604" t="n">
-        <v>1435.543436192616</v>
-      </c>
-      <c r="S604" t="n">
-        <v>1500.325054579304</v>
-      </c>
-    </row>
-    <row r="605">
-      <c r="A605" t="n">
-        <v>1046.165026244933</v>
-      </c>
-      <c r="C605" t="n">
-        <v>662.9442155562589</v>
-      </c>
-      <c r="E605" t="n">
-        <v>1648.716633388023</v>
-      </c>
-      <c r="G605" t="n">
-        <v>1436.344106894996</v>
-      </c>
-      <c r="I605" t="n">
-        <v>430.340326397527</v>
-      </c>
-      <c r="K605" t="n">
-        <v>-972.3078570202688</v>
-      </c>
-      <c r="M605" t="n">
-        <v>988.5676057394903</v>
-      </c>
-      <c r="O605" t="n">
-        <v>373.4080385813741</v>
-      </c>
-      <c r="Q605" t="n">
-        <v>1436.250093923853</v>
-      </c>
-      <c r="S605" t="n">
-        <v>1501.031787020658</v>
-      </c>
-    </row>
-    <row r="606">
-      <c r="A606" t="n">
-        <v>1046.595366571331</v>
-      </c>
-      <c r="C606" t="n">
-        <v>661.9719076992386</v>
-      </c>
-      <c r="E606" t="n">
-        <v>1649.705200993762</v>
-      </c>
-      <c r="G606" t="n">
-        <v>1436.717514933578</v>
-      </c>
-      <c r="I606" t="n">
-        <v>431.10784708756</v>
-      </c>
-      <c r="K606" t="n">
-        <v>-972.2220977209872</v>
-      </c>
-      <c r="M606" t="n">
-        <v>988.5745434346518</v>
-      </c>
-      <c r="O606" t="n">
-        <v>374.0118138730395</v>
-      </c>
-      <c r="Q606" t="n">
-        <v>1436.956744551328</v>
-      </c>
-      <c r="S606" t="n">
-        <v>1501.738526189997</v>
-      </c>
-    </row>
-    <row r="607">
-      <c r="A607" t="n">
-        <v>1047.026474418419</v>
-      </c>
-      <c r="C607" t="n">
-        <v>660.9996856015176</v>
-      </c>
-      <c r="E607" t="n">
-        <v>1650.693775537197</v>
-      </c>
-      <c r="G607" t="n">
-        <v>1437.091526747451</v>
-      </c>
-      <c r="I607" t="n">
-        <v>431.8743386506867</v>
-      </c>
-      <c r="K607" t="n">
-        <v>-972.1359211146137</v>
-      </c>
-      <c r="M607" t="n">
-        <v>988.5813972400683</v>
-      </c>
-      <c r="O607" t="n">
-        <v>374.6151504155932</v>
-      </c>
-      <c r="Q607" t="n">
-        <v>1437.663387962111</v>
-      </c>
-      <c r="S607" t="n">
-        <v>1502.445272196956</v>
-      </c>
-    </row>
-    <row r="608">
-      <c r="A608" t="n">
-        <v>1047.458348757069</v>
-      </c>
-      <c r="C608" t="n">
-        <v>660.027549680403</v>
-      </c>
-      <c r="E608" t="n">
-        <v>1651.682356934437</v>
-      </c>
-      <c r="G608" t="n">
-        <v>1437.466141897866</v>
-      </c>
-      <c r="I608" t="n">
-        <v>432.6398000487188</v>
-      </c>
-      <c r="K608" t="n">
-        <v>-972.0493240076848</v>
-      </c>
-      <c r="M608" t="n">
-        <v>988.5881659231472</v>
-      </c>
-      <c r="O608" t="n">
-        <v>375.2180481476444</v>
-      </c>
-      <c r="Q608" t="n">
-        <v>1438.370024040958</v>
-      </c>
-      <c r="S608" t="n">
-        <v>1503.152025153437</v>
-      </c>
-    </row>
-    <row r="609">
-      <c r="A609" t="n">
-        <v>1047.890988557118</v>
-      </c>
-      <c r="C609" t="n">
-        <v>659.0555003563953</v>
-      </c>
-      <c r="E609" t="n">
-        <v>1652.67094510036</v>
-      </c>
-      <c r="G609" t="n">
-        <v>1437.841359946014</v>
-      </c>
-      <c r="I609" t="n">
-        <v>433.4042302261878</v>
-      </c>
-      <c r="K609" t="n">
-        <v>-971.9623031603533</v>
-      </c>
-      <c r="M609" t="n">
-        <v>988.5948482101412</v>
-      </c>
-      <c r="O609" t="n">
-        <v>375.820507013259</v>
-      </c>
-      <c r="Q609" t="n">
-        <v>1439.076652670242</v>
-      </c>
-      <c r="S609" t="n">
-        <v>1503.858785173688</v>
-      </c>
-    </row>
-    <row r="610">
-      <c r="A610" t="n">
-        <v>1048.324392787344</v>
-      </c>
-      <c r="C610" t="n">
-        <v>658.083538053235</v>
-      </c>
-      <c r="E610" t="n">
-        <v>1653.65953994857</v>
-      </c>
-      <c r="G610" t="n">
-        <v>1438.217180453027</v>
-      </c>
-      <c r="I610" t="n">
-        <v>434.1676281119362</v>
-      </c>
-      <c r="K610" t="n">
-        <v>-971.8748552850229</v>
-      </c>
-      <c r="M610" t="n">
-        <v>988.6014427893315</v>
-      </c>
-      <c r="O610" t="n">
-        <v>376.4225269617327</v>
-      </c>
-      <c r="Q610" t="n">
-        <v>1439.783273729883</v>
-      </c>
-      <c r="S610" t="n">
-        <v>1504.565552374371</v>
-      </c>
-    </row>
-    <row r="611">
-      <c r="A611" t="n">
-        <v>1048.758560415456</v>
-      </c>
-      <c r="C611" t="n">
-        <v>657.11166319795</v>
-      </c>
-      <c r="E611" t="n">
-        <v>1654.64814139136</v>
-      </c>
-      <c r="G611" t="n">
-        <v>1438.593602979989</v>
-      </c>
-      <c r="I611" t="n">
-        <v>434.9299926170715</v>
-      </c>
-      <c r="K611" t="n">
-        <v>-971.7869770448715</v>
-      </c>
-      <c r="M611" t="n">
-        <v>988.6079483032972</v>
-      </c>
-      <c r="O611" t="n">
-        <v>377.0241079469088</v>
-      </c>
-      <c r="Q611" t="n">
-        <v>1440.489887097271</v>
-      </c>
-      <c r="S611" t="n">
-        <v>1505.272326874635</v>
-      </c>
-    </row>
-    <row r="612">
-      <c r="A612" t="n">
-        <v>1049.193490408073</v>
-      </c>
-      <c r="C612" t="n">
-        <v>656.1398762209051</v>
-      </c>
-      <c r="E612" t="n">
-        <v>1655.636749339663</v>
-      </c>
-      <c r="G612" t="n">
-        <v>1438.970627087936</v>
-      </c>
-      <c r="I612" t="n">
-        <v>435.6913226336019</v>
-      </c>
-      <c r="K612" t="n">
-        <v>-971.6986650540775</v>
-      </c>
-      <c r="M612" t="n">
-        <v>988.6143633509619</v>
-      </c>
-      <c r="O612" t="n">
-        <v>377.6252499258135</v>
-      </c>
-      <c r="Q612" t="n">
-        <v>1441.196492647187</v>
-      </c>
-      <c r="S612" t="n">
-        <v>1505.979108796194</v>
-      </c>
-    </row>
-    <row r="613">
-      <c r="A613" t="n">
-        <v>1049.629181730707</v>
-      </c>
-      <c r="C613" t="n">
-        <v>655.168177555851</v>
-      </c>
-      <c r="E613" t="n">
-        <v>1656.625363703014</v>
-      </c>
-      <c r="G613" t="n">
-        <v>1439.348252337862</v>
-      </c>
-      <c r="I613" t="n">
-        <v>436.4516170344359</v>
-      </c>
-      <c r="K613" t="n">
-        <v>-971.6099158746374</v>
-      </c>
-      <c r="M613" t="n">
-        <v>988.6206864855467</v>
-      </c>
-      <c r="O613" t="n">
-        <v>378.2259528627492</v>
-      </c>
-      <c r="Q613" t="n">
-        <v>1441.90309025172</v>
-      </c>
-      <c r="S613" t="n">
-        <v>1506.685898263412</v>
-      </c>
-    </row>
-    <row r="614">
-      <c r="A614" t="n">
-        <v>1050.065633347741</v>
-      </c>
-      <c r="C614" t="n">
-        <v>654.1965676399764</v>
-      </c>
-      <c r="E614" t="n">
-        <v>1657.613984389499</v>
-      </c>
-      <c r="G614" t="n">
-        <v>1439.726478290724</v>
-      </c>
-      <c r="I614" t="n">
-        <v>437.2108746717913</v>
-      </c>
-      <c r="K614" t="n">
-        <v>-971.5207260140915</v>
-      </c>
-      <c r="M614" t="n">
-        <v>988.6269162109329</v>
-      </c>
-      <c r="O614" t="n">
-        <v>378.8262167252014</v>
-      </c>
-      <c r="Q614" t="n">
-        <v>1442.609679780186</v>
-      </c>
-      <c r="S614" t="n">
-        <v>1507.39269540338</v>
-      </c>
-    </row>
-    <row r="615">
-      <c r="A615" t="n">
-        <v>1050.502844222413</v>
-      </c>
-      <c r="C615" t="n">
-        <v>653.2250469139623</v>
-      </c>
-      <c r="E615" t="n">
-        <v>1658.60261130571</v>
-      </c>
-      <c r="G615" t="n">
-        <v>1440.10530450745</v>
-      </c>
-      <c r="I615" t="n">
-        <v>437.9690943760579</v>
-      </c>
-      <c r="K615" t="n">
-        <v>-971.4310919264335</v>
-      </c>
-      <c r="M615" t="n">
-        <v>988.63305098007</v>
-      </c>
-      <c r="O615" t="n">
-        <v>379.4260414856581</v>
-      </c>
-      <c r="Q615" t="n">
-        <v>1443.316261099035</v>
-      </c>
-      <c r="S615" t="n">
-        <v>1508.099500346008</v>
-      </c>
-    </row>
-    <row r="616">
-      <c r="A616" t="n">
-        <v>1050.940813316789</v>
-      </c>
-      <c r="C616" t="n">
-        <v>652.2536158220358</v>
-      </c>
-      <c r="E616" t="n">
-        <v>1659.59124435669</v>
-      </c>
-      <c r="G616" t="n">
-        <v>1440.484730548935</v>
-      </c>
-      <c r="I616" t="n">
-        <v>438.7262749551155</v>
-      </c>
-      <c r="K616" t="n">
-        <v>-971.3410100073361</v>
-      </c>
-      <c r="M616" t="n">
-        <v>988.6390891958854</v>
-      </c>
-      <c r="O616" t="n">
-        <v>380.0254271211543</v>
-      </c>
-      <c r="Q616" t="n">
-        <v>1444.022834071759</v>
-      </c>
-      <c r="S616" t="n">
-        <v>1508.806313224116</v>
-      </c>
-    </row>
-    <row r="617">
-      <c r="A617" t="n">
-        <v>1051.379539591744</v>
-      </c>
-      <c r="C617" t="n">
-        <v>651.2822748120285</v>
-      </c>
-      <c r="E617" t="n">
-        <v>1660.579883445886</v>
-      </c>
-      <c r="G617" t="n">
-        <v>1440.864755976056</v>
-      </c>
-      <c r="I617" t="n">
-        <v>439.4824151934245</v>
-      </c>
-      <c r="K617" t="n">
-        <v>-971.2504765949461</v>
-      </c>
-      <c r="M617" t="n">
-        <v>988.645029203326</v>
-      </c>
-      <c r="O617" t="n">
-        <v>380.6243736146371</v>
-      </c>
-      <c r="Q617" t="n">
-        <v>1444.729398558802</v>
-      </c>
-      <c r="S617" t="n">
-        <v>1509.513134173524</v>
-      </c>
-    </row>
-    <row r="618">
-      <c r="A618" t="n">
-        <v>1051.819022006938</v>
-      </c>
-      <c r="C618" t="n">
-        <v>650.3110243354336</v>
-      </c>
-      <c r="E618" t="n">
-        <v>1661.56852847509</v>
-      </c>
-      <c r="G618" t="n">
-        <v>1441.245380349671</v>
-      </c>
-      <c r="I618" t="n">
-        <v>440.2375138490697</v>
-      </c>
-      <c r="K618" t="n">
-        <v>-971.1594879670429</v>
-      </c>
-      <c r="M618" t="n">
-        <v>988.6508692907228</v>
-      </c>
-      <c r="O618" t="n">
-        <v>381.2228809515545</v>
-      </c>
-      <c r="Q618" t="n">
-        <v>1445.435954417447</v>
-      </c>
-      <c r="S618" t="n">
-        <v>1510.219963333161</v>
-      </c>
-    </row>
-    <row r="619">
-      <c r="A619" t="n">
-        <v>1052.259259520787</v>
-      </c>
-      <c r="C619" t="n">
-        <v>649.3398648474665</v>
-      </c>
-      <c r="E619" t="n">
-        <v>1662.55717934438</v>
-      </c>
-      <c r="G619" t="n">
-        <v>1441.626603230623</v>
-      </c>
-      <c r="I619" t="n">
-        <v>440.9915696542157</v>
-      </c>
-      <c r="K619" t="n">
-        <v>-971.0680403373999</v>
-      </c>
-      <c r="M619" t="n">
-        <v>988.6566076881991</v>
-      </c>
-      <c r="O619" t="n">
-        <v>381.8209491237212</v>
-      </c>
-      <c r="Q619" t="n">
-        <v>1446.142501501721</v>
-      </c>
-      <c r="S619" t="n">
-        <v>1510.926800845159</v>
-      </c>
-    </row>
-    <row r="620">
-      <c r="A620" t="n">
-        <v>1052.700251090441</v>
-      </c>
-      <c r="C620" t="n">
-        <v>648.3687968071291</v>
-      </c>
-      <c r="E620" t="n">
-        <v>1663.545835952069</v>
-      </c>
-      <c r="G620" t="n">
-        <v>1442.008424179746</v>
-      </c>
-      <c r="I620" t="n">
-        <v>441.7445813135146</v>
-      </c>
-      <c r="K620" t="n">
-        <v>-970.9761298561261</v>
-      </c>
-      <c r="M620" t="n">
-        <v>988.6622425603946</v>
-      </c>
-      <c r="O620" t="n">
-        <v>382.4185781277265</v>
-      </c>
-      <c r="Q620" t="n">
-        <v>1446.849039662285</v>
-      </c>
-      <c r="S620" t="n">
-        <v>1511.633646854965</v>
-      </c>
-    </row>
-    <row r="621">
-      <c r="A621" t="n">
-        <v>1053.141995671754</v>
-      </c>
-      <c r="C621" t="n">
-        <v>647.397820677273</v>
-      </c>
-      <c r="E621" t="n">
-        <v>1664.534498194629</v>
-      </c>
-      <c r="G621" t="n">
-        <v>1442.390842757874</v>
-      </c>
-      <c r="I621" t="n">
-        <v>442.4965475016052</v>
-      </c>
-      <c r="K621" t="n">
-        <v>-970.8837526054594</v>
-      </c>
-      <c r="M621" t="n">
-        <v>988.6677720096486</v>
-      </c>
-      <c r="O621" t="n">
-        <v>383.015767963343</v>
-      </c>
-      <c r="Q621" t="n">
-        <v>1447.55556874631</v>
-      </c>
-      <c r="S621" t="n">
-        <v>1512.340501511456</v>
-      </c>
-    </row>
-    <row r="622">
-      <c r="A622" t="n">
-        <v>1053.584492219256</v>
-      </c>
-      <c r="C622" t="n">
-        <v>646.4269369246675</v>
-      </c>
-      <c r="E622" t="n">
-        <v>1665.523165966639</v>
-      </c>
-      <c r="G622" t="n">
-        <v>1442.773858525837</v>
-      </c>
-      <c r="I622" t="n">
-        <v>443.2474668624309</v>
-      </c>
-      <c r="K622" t="n">
-        <v>-970.7909045993119</v>
-      </c>
-      <c r="M622" t="n">
-        <v>988.673194066223</v>
-      </c>
-      <c r="O622" t="n">
-        <v>383.6125186362551</v>
-      </c>
-      <c r="Q622" t="n">
-        <v>1448.262088597369</v>
-      </c>
-      <c r="S622" t="n">
-        <v>1513.047364967056</v>
-      </c>
-    </row>
-    <row r="623">
-      <c r="A623" t="n">
-        <v>1054.027739686118</v>
-      </c>
-      <c r="C623" t="n">
-        <v>645.4561460200682</v>
-      </c>
-      <c r="E623" t="n">
-        <v>1666.511839160705</v>
-      </c>
-      <c r="G623" t="n">
-        <v>1443.157471044474</v>
-      </c>
-      <c r="I623" t="n">
-        <v>443.9973380076481</v>
-      </c>
-      <c r="K623" t="n">
-        <v>-970.6975817783814</v>
-      </c>
-      <c r="M623" t="n">
-        <v>988.6785066919401</v>
-      </c>
-      <c r="O623" t="n">
-        <v>384.2088301560125</v>
-      </c>
-      <c r="Q623" t="n">
-        <v>1448.968599055301</v>
-      </c>
-      <c r="S623" t="n">
-        <v>1513.754237377856</v>
-      </c>
-    </row>
-    <row r="624">
-      <c r="A624" t="n">
-        <v>1054.471737024126</v>
-      </c>
-      <c r="C624" t="n">
-        <v>644.4854484382898</v>
-      </c>
-      <c r="E624" t="n">
-        <v>1667.500517667397</v>
-      </c>
-      <c r="G624" t="n">
-        <v>1443.54167987463</v>
-      </c>
-      <c r="I624" t="n">
-        <v>444.7461595152618</v>
-      </c>
-      <c r="K624" t="n">
-        <v>-970.6037800103786</v>
-      </c>
-      <c r="M624" t="n">
-        <v>988.6837077713153</v>
-      </c>
-      <c r="O624" t="n">
-        <v>384.8047025360302</v>
-      </c>
-      <c r="Q624" t="n">
-        <v>1449.675099956089</v>
-      </c>
-      <c r="S624" t="n">
-        <v>1514.461118903749</v>
-      </c>
-    </row>
-    <row r="625">
-      <c r="A625" t="n">
-        <v>1054.916483183641</v>
-      </c>
-      <c r="C625" t="n">
-        <v>643.5148446582795</v>
-      </c>
-      <c r="E625" t="n">
-        <v>1668.489201375168</v>
-      </c>
-      <c r="G625" t="n">
-        <v>1443.926484577166</v>
-      </c>
-      <c r="I625" t="n">
-        <v>445.4939299262151</v>
-      </c>
-      <c r="K625" t="n">
-        <v>-970.5094950842295</v>
-      </c>
-      <c r="M625" t="n">
-        <v>988.68879511042</v>
-      </c>
-      <c r="O625" t="n">
-        <v>385.400135796317</v>
-      </c>
-      <c r="Q625" t="n">
-        <v>1450.381591131713</v>
-      </c>
-      <c r="S625" t="n">
-        <v>1515.168009708563</v>
-      </c>
-    </row>
-    <row r="626">
-      <c r="A626" t="n">
-        <v>1055.361977113567</v>
-      </c>
-      <c r="C626" t="n">
-        <v>642.5443351631952</v>
-      </c>
-      <c r="E626" t="n">
-        <v>1669.477890170278</v>
-      </c>
-      <c r="G626" t="n">
-        <v>1444.311884712962</v>
-      </c>
-      <c r="I626" t="n">
-        <v>446.2406477441618</v>
-      </c>
-      <c r="K626" t="n">
-        <v>-970.4147227095063</v>
-      </c>
-      <c r="M626" t="n">
-        <v>988.6937664339257</v>
-      </c>
-      <c r="O626" t="n">
-        <v>385.9951299580189</v>
-      </c>
-      <c r="Q626" t="n">
-        <v>1451.088072410015</v>
-      </c>
-      <c r="S626" t="n">
-        <v>1515.874909960201</v>
-      </c>
-    </row>
-    <row r="627">
-      <c r="A627" t="n">
-        <v>1055.808217761312</v>
-      </c>
-      <c r="C627" t="n">
-        <v>641.5739204404857</v>
-      </c>
-      <c r="E627" t="n">
-        <v>1670.466583936712</v>
-      </c>
-      <c r="G627" t="n">
-        <v>1444.69787984292</v>
-      </c>
-      <c r="I627" t="n">
-        <v>446.9863114331929</v>
-      </c>
-      <c r="K627" t="n">
-        <v>-970.3194585115398</v>
-      </c>
-      <c r="M627" t="n">
-        <v>988.6986193789653</v>
-      </c>
-      <c r="O627" t="n">
-        <v>386.5896850500121</v>
-      </c>
-      <c r="Q627" t="n">
-        <v>1451.794543614542</v>
-      </c>
-      <c r="S627" t="n">
-        <v>1516.581819830796</v>
-      </c>
-    </row>
-    <row r="628">
-      <c r="A628" t="n">
-        <v>1056.255204072745</v>
-      </c>
-      <c r="C628" t="n">
-        <v>640.6036009819742</v>
-      </c>
-      <c r="E628" t="n">
-        <v>1671.455282556091</v>
-      </c>
-      <c r="G628" t="n">
-        <v>1445.08446952797</v>
-      </c>
-      <c r="I628" t="n">
-        <v>447.7309194155623</v>
-      </c>
-      <c r="K628" t="n">
-        <v>-970.223698029713</v>
-      </c>
-      <c r="M628" t="n">
-        <v>988.7033514910399</v>
-      </c>
-      <c r="O628" t="n">
-        <v>387.1838011011732</v>
-      </c>
-      <c r="Q628" t="n">
-        <v>1452.501004564388</v>
-      </c>
-      <c r="S628" t="n">
-        <v>1517.28873949686</v>
-      </c>
-    </row>
-    <row r="629">
-      <c r="A629" t="n">
-        <v>1056.70293499216</v>
-      </c>
-      <c r="C629" t="n">
-        <v>639.6333772839445</v>
-      </c>
-      <c r="E629" t="n">
-        <v>1672.443985907582</v>
-      </c>
-      <c r="G629" t="n">
-        <v>1445.471653329071</v>
-      </c>
-      <c r="I629" t="n">
-        <v>448.4744700687315</v>
-      </c>
-      <c r="K629" t="n">
-        <v>-970.1274367132555</v>
-      </c>
-      <c r="M629" t="n">
-        <v>988.7079602219728</v>
-      </c>
-      <c r="O629" t="n">
-        <v>387.7774781483367</v>
-      </c>
-      <c r="Q629" t="n">
-        <v>1453.207455074031</v>
-      </c>
-      <c r="S629" t="n">
-        <v>1517.99566913945</v>
-      </c>
-    </row>
-    <row r="630">
-      <c r="A630" t="n">
-        <v>1057.151409462229</v>
-      </c>
-      <c r="C630" t="n">
-        <v>638.6632498472312</v>
-      </c>
-      <c r="E630" t="n">
-        <v>1673.432693867804</v>
-      </c>
-      <c r="G630" t="n">
-        <v>1445.859430807219</v>
-      </c>
-      <c r="I630" t="n">
-        <v>449.2169617246873</v>
-      </c>
-      <c r="K630" t="n">
-        <v>-970.0306699169232</v>
-      </c>
-      <c r="M630" t="n">
-        <v>988.7124429226333</v>
-      </c>
-      <c r="O630" t="n">
-        <v>388.3707162292467</v>
-      </c>
-      <c r="Q630" t="n">
-        <v>1453.913894953157</v>
-      </c>
-      <c r="S630" t="n">
-        <v>1518.702608944343</v>
-      </c>
-    </row>
-    <row r="631">
-      <c r="A631" t="n">
-        <v>1057.600626423954</v>
-      </c>
-      <c r="C631" t="n">
-        <v>637.6932191773143</v>
-      </c>
-      <c r="E631" t="n">
-        <v>1674.421406310727</v>
-      </c>
-      <c r="G631" t="n">
-        <v>1446.247801523449</v>
-      </c>
-      <c r="I631" t="n">
-        <v>449.9583926653941</v>
-      </c>
-      <c r="K631" t="n">
-        <v>-969.9333928982696</v>
-      </c>
-      <c r="M631" t="n">
-        <v>988.716796837025</v>
-      </c>
-      <c r="O631" t="n">
-        <v>388.9635153877862</v>
-      </c>
-      <c r="Q631" t="n">
-        <v>1454.620324006474</v>
-      </c>
-      <c r="S631" t="n">
-        <v>1519.409559102213</v>
-      </c>
-    </row>
-    <row r="632">
-      <c r="A632" t="n">
-        <v>1058.050584816619</v>
-      </c>
-      <c r="C632" t="n">
-        <v>636.723285784416</v>
-      </c>
-      <c r="E632" t="n">
-        <v>1675.410123107564</v>
-      </c>
-      <c r="G632" t="n">
-        <v>1446.636765038837</v>
-      </c>
-      <c r="I632" t="n">
-        <v>450.6987611225668</v>
-      </c>
-      <c r="K632" t="n">
-        <v>-969.8356008125302</v>
-      </c>
-      <c r="M632" t="n">
-        <v>988.7210191002396</v>
-      </c>
-      <c r="O632" t="n">
-        <v>389.55587566943</v>
-      </c>
-      <c r="Q632" t="n">
-        <v>1455.326742033525</v>
-      </c>
-      <c r="S632" t="n">
-        <v>1520.116519808822</v>
-      </c>
-    </row>
-    <row r="633">
-      <c r="A633" t="n">
-        <v>1058.501283577742</v>
-      </c>
-      <c r="C633" t="n">
-        <v>635.7534501836035</v>
-      </c>
-      <c r="E633" t="n">
-        <v>1676.398844126664</v>
-      </c>
-      <c r="G633" t="n">
-        <v>1447.026320914506</v>
-      </c>
-      <c r="I633" t="n">
-        <v>451.4380652722139</v>
-      </c>
-      <c r="K633" t="n">
-        <v>-969.7372887088704</v>
-      </c>
-      <c r="M633" t="n">
-        <v>988.7251067289071</v>
-      </c>
-      <c r="O633" t="n">
-        <v>390.1477971235181</v>
-      </c>
-      <c r="Q633" t="n">
-        <v>1456.033148828479</v>
-      </c>
-      <c r="S633" t="n">
-        <v>1520.823491265221</v>
-      </c>
-    </row>
-    <row r="634">
-      <c r="A634" t="n">
-        <v>1058.952721643014</v>
-      </c>
-      <c r="C634" t="n">
-        <v>634.7837128948946</v>
-      </c>
-      <c r="E634" t="n">
-        <v>1677.387569233393</v>
-      </c>
-      <c r="G634" t="n">
-        <v>1447.416468711629</v>
-      </c>
-      <c r="I634" t="n">
-        <v>452.1763032341823</v>
-      </c>
-      <c r="K634" t="n">
-        <v>-969.6384515256113</v>
-      </c>
-      <c r="M634" t="n">
-        <v>988.7290566168758</v>
-      </c>
-      <c r="O634" t="n">
-        <v>390.7392798028013</v>
-      </c>
-      <c r="Q634" t="n">
-        <v>1456.739544179921</v>
-      </c>
-      <c r="S634" t="n">
-        <v>1521.530473677958</v>
-      </c>
-    </row>
-    <row r="635">
-      <c r="A635" t="n">
-        <v>1059.404897946248</v>
-      </c>
-      <c r="C635" t="n">
-        <v>633.814074443369</v>
-      </c>
-      <c r="E635" t="n">
-        <v>1678.37629829001</v>
-      </c>
-      <c r="G635" t="n">
-        <v>1447.807207991432</v>
-      </c>
-      <c r="I635" t="n">
-        <v>452.9134730669284</v>
-      </c>
-      <c r="K635" t="n">
-        <v>-969.5390840844311</v>
-      </c>
-      <c r="M635" t="n">
-        <v>988.7328655297551</v>
-      </c>
-      <c r="O635" t="n">
-        <v>391.3303237634409</v>
-      </c>
-      <c r="Q635" t="n">
-        <v>1457.445927870627</v>
-      </c>
-      <c r="S635" t="n">
-        <v>1522.237467259303</v>
-      </c>
-    </row>
-    <row r="636">
-      <c r="A636" t="n">
-        <v>1059.857811419315</v>
-      </c>
-      <c r="C636" t="n">
-        <v>632.8445353592846</v>
-      </c>
-      <c r="E636" t="n">
-        <v>1679.36503115554</v>
-      </c>
-      <c r="G636" t="n">
-        <v>1448.198538315196</v>
-      </c>
-      <c r="I636" t="n">
-        <v>453.6495727663805</v>
-      </c>
-      <c r="K636" t="n">
-        <v>-969.4391810862726</v>
-      </c>
-      <c r="M636" t="n">
-        <v>988.7365300940019</v>
-      </c>
-      <c r="O636" t="n">
-        <v>391.9209290625076</v>
-      </c>
-      <c r="Q636" t="n">
-        <v>1458.152299677329</v>
-      </c>
-      <c r="S636" t="n">
-        <v>1522.944472227477</v>
-      </c>
-    </row>
-    <row r="637">
-      <c r="A637" t="n">
-        <v>1060.311460992081</v>
-      </c>
-      <c r="C637" t="n">
-        <v>631.8750961781983</v>
-      </c>
-      <c r="E637" t="n">
-        <v>1680.353767685634</v>
-      </c>
-      <c r="G637" t="n">
-        <v>1448.590459244258</v>
-      </c>
-      <c r="I637" t="n">
-        <v>454.3846002595728</v>
-      </c>
-      <c r="K637" t="n">
-        <v>-969.3387371044082</v>
-      </c>
-      <c r="M637" t="n">
-        <v>988.7400467919178</v>
-      </c>
-      <c r="O637" t="n">
-        <v>392.5110957613924</v>
-      </c>
-      <c r="Q637" t="n">
-        <v>1458.858659370459</v>
-      </c>
-      <c r="S637" t="n">
-        <v>1523.651488806901</v>
-      </c>
-    </row>
-    <row r="638">
-      <c r="A638" t="n">
-        <v>1060.765845592341</v>
-      </c>
-      <c r="C638" t="n">
-        <v>630.9057574410939</v>
-      </c>
-      <c r="E638" t="n">
-        <v>1681.342507732426</v>
-      </c>
-      <c r="G638" t="n">
-        <v>1448.98297034002</v>
-      </c>
-      <c r="I638" t="n">
-        <v>455.1185534035085</v>
-      </c>
-      <c r="K638" t="n">
-        <v>-969.2377465798927</v>
-      </c>
-      <c r="M638" t="n">
-        <v>988.7434119546015</v>
-      </c>
-      <c r="O638" t="n">
-        <v>393.1008239217135</v>
-      </c>
-      <c r="Q638" t="n">
-        <v>1459.565006713892</v>
-      </c>
-      <c r="S638" t="n">
-        <v>1524.358517228455</v>
-      </c>
-    </row>
-    <row r="639">
-      <c r="A639" t="n">
-        <v>1061.220964145745</v>
-      </c>
-      <c r="C639" t="n">
-        <v>629.936519694514</v>
-      </c>
-      <c r="E639" t="n">
-        <v>1682.33125114438</v>
-      </c>
-      <c r="G639" t="n">
-        <v>1449.376071163941</v>
-      </c>
-      <c r="I639" t="n">
-        <v>455.8514299797025</v>
-      </c>
-      <c r="K639" t="n">
-        <v>-969.1362038137186</v>
-      </c>
-      <c r="M639" t="n">
-        <v>988.7466217501242</v>
-      </c>
-      <c r="O639" t="n">
-        <v>393.6901136084998</v>
-      </c>
-      <c r="Q639" t="n">
-        <v>1460.271341464666</v>
-      </c>
-      <c r="S639" t="n">
-        <v>1525.06555772975</v>
-      </c>
-    </row>
-    <row r="640">
-      <c r="A640" t="n">
-        <v>1061.676815575724</v>
-      </c>
-      <c r="C640" t="n">
-        <v>628.9673834907003</v>
-      </c>
-      <c r="E640" t="n">
-        <v>1683.31999776613</v>
-      </c>
-      <c r="G640" t="n">
-        <v>1449.76976127755</v>
-      </c>
-      <c r="I640" t="n">
-        <v>456.5832276909987</v>
-      </c>
-      <c r="K640" t="n">
-        <v>-969.0341029598812</v>
-      </c>
-      <c r="M640" t="n">
-        <v>988.7496721764819</v>
-      </c>
-      <c r="O640" t="n">
-        <v>394.2789648863254</v>
-      </c>
-      <c r="Q640" t="n">
-        <v>1460.977663372682</v>
-      </c>
-      <c r="S640" t="n">
-        <v>1525.772610555424</v>
-      </c>
-    </row>
-    <row r="641">
-      <c r="A641" t="n">
-        <v>1062.133398803415</v>
-      </c>
-      <c r="C641" t="n">
-        <v>627.9983493877404</v>
-      </c>
-      <c r="E641" t="n">
-        <v>1684.308747438307</v>
-      </c>
-      <c r="G641" t="n">
-        <v>1450.164040242436</v>
-      </c>
-      <c r="I641" t="n">
-        <v>457.3139441536114</v>
-      </c>
-      <c r="K641" t="n">
-        <v>-968.9314380202632</v>
-      </c>
-      <c r="M641" t="n">
-        <v>988.752559049999</v>
-      </c>
-      <c r="O641" t="n">
-        <v>394.8673778215834</v>
-      </c>
-      <c r="Q641" t="n">
-        <v>1461.683972180402</v>
-      </c>
-      <c r="S641" t="n">
-        <v>1526.479675957443</v>
-      </c>
-    </row>
-    <row r="642">
-      <c r="A642" t="n">
-        <v>1062.590712747569</v>
-      </c>
-      <c r="C642" t="n">
-        <v>627.0294179497201</v>
-      </c>
-      <c r="E642" t="n">
-        <v>1685.297499997357</v>
-      </c>
-      <c r="G642" t="n">
-        <v>1450.558907620258</v>
-      </c>
-      <c r="I642" t="n">
-        <v>458.0435768989446</v>
-      </c>
-      <c r="K642" t="n">
-        <v>-968.8282028326967</v>
-      </c>
-      <c r="M642" t="n">
-        <v>988.7552779950965</v>
-      </c>
-      <c r="O642" t="n">
-        <v>395.4553524799849</v>
-      </c>
-      <c r="Q642" t="n">
-        <v>1462.390267622512</v>
-      </c>
-      <c r="S642" t="n">
-        <v>1527.186754195428</v>
-      </c>
-    </row>
-    <row r="643">
-      <c r="A643" t="n">
-        <v>1063.048756324468</v>
-      </c>
-      <c r="C643" t="n">
-        <v>626.0605897468874</v>
-      </c>
-      <c r="E643" t="n">
-        <v>1686.286255275352</v>
-      </c>
-      <c r="G643" t="n">
-        <v>1450.954362972738</v>
-      </c>
-      <c r="I643" t="n">
-        <v>458.7721233604043</v>
-      </c>
-      <c r="K643" t="n">
-        <v>-968.724391067326</v>
-      </c>
-      <c r="M643" t="n">
-        <v>988.7578244331507</v>
-      </c>
-      <c r="O643" t="n">
-        <v>396.0428889276955</v>
-      </c>
-      <c r="Q643" t="n">
-        <v>1463.096549425574</v>
-      </c>
-      <c r="S643" t="n">
-        <v>1527.893845537</v>
-      </c>
-    </row>
-    <row r="644">
-      <c r="A644" t="n">
-        <v>1063.507528447828</v>
-      </c>
-      <c r="C644" t="n">
-        <v>625.0918653558201</v>
-      </c>
-      <c r="E644" t="n">
-        <v>1687.275013099785</v>
-      </c>
-      <c r="G644" t="n">
-        <v>1451.350405861665</v>
-      </c>
-      <c r="I644" t="n">
-        <v>459.499580873171</v>
-      </c>
-      <c r="K644" t="n">
-        <v>-968.6199962121691</v>
-      </c>
-      <c r="M644" t="n">
-        <v>988.7601935706698</v>
-      </c>
-      <c r="O644" t="n">
-        <v>396.6299872292893</v>
-      </c>
-      <c r="Q644" t="n">
-        <v>1463.802817307659</v>
-      </c>
-      <c r="S644" t="n">
-        <v>1528.600950258143</v>
-      </c>
-    </row>
-    <row r="645">
-      <c r="A645" t="n">
-        <v>1063.967028028701</v>
-      </c>
-      <c r="C645" t="n">
-        <v>624.1232453596079</v>
-      </c>
-      <c r="E645" t="n">
-        <v>1688.263773293356</v>
-      </c>
-      <c r="G645" t="n">
-        <v>1451.747035848895</v>
-      </c>
-      <c r="I645" t="n">
-        <v>460.2259466669238</v>
-      </c>
-      <c r="K645" t="n">
-        <v>-968.5150115681154</v>
-      </c>
-      <c r="M645" t="n">
-        <v>988.762380381786</v>
-      </c>
-      <c r="O645" t="n">
-        <v>397.2166474486585</v>
-      </c>
-      <c r="Q645" t="n">
-        <v>1464.509070977951</v>
-      </c>
-      <c r="S645" t="n">
-        <v>1529.308068643592</v>
-      </c>
-    </row>
-    <row r="646">
-      <c r="A646" t="n">
-        <v>1064.427253975368</v>
-      </c>
-      <c r="C646" t="n">
-        <v>623.1547303480398</v>
-      </c>
-      <c r="E646" t="n">
-        <v>1689.252535673738</v>
-      </c>
-      <c r="G646" t="n">
-        <v>1452.144252496343</v>
-      </c>
-      <c r="I646" t="n">
-        <v>460.9512178578825</v>
-      </c>
-      <c r="K646" t="n">
-        <v>-968.4094302344874</v>
-      </c>
-      <c r="M646" t="n">
-        <v>988.7643795989334</v>
-      </c>
-      <c r="O646" t="n">
-        <v>397.8028696453748</v>
-      </c>
-      <c r="Q646" t="n">
-        <v>1465.215310136328</v>
-      </c>
-      <c r="S646" t="n">
-        <v>1530.015200987246</v>
-      </c>
-    </row>
-    <row r="647">
-      <c r="A647" t="n">
-        <v>1064.888205193226</v>
-      </c>
-      <c r="C647" t="n">
-        <v>622.1863209178053</v>
-      </c>
-      <c r="E647" t="n">
-        <v>1690.241300053337</v>
-      </c>
-      <c r="G647" t="n">
-        <v>1452.542055365989</v>
-      </c>
-      <c r="I647" t="n">
-        <v>461.6753914428955</v>
-      </c>
-      <c r="K647" t="n">
-        <v>-968.3032451018789</v>
-      </c>
-      <c r="M647" t="n">
-        <v>988.7661856932937</v>
-      </c>
-      <c r="O647" t="n">
-        <v>398.388653877646</v>
-      </c>
-      <c r="Q647" t="n">
-        <v>1465.921534472922</v>
-      </c>
-      <c r="S647" t="n">
-        <v>1530.722347592602</v>
-      </c>
-    </row>
-    <row r="648">
-      <c r="A648" t="n">
-        <v>1065.349880584669</v>
-      </c>
-      <c r="C648" t="n">
-        <v>621.2180176727035</v>
-      </c>
-      <c r="E648" t="n">
-        <v>1691.23006623903</v>
-      </c>
-      <c r="G648" t="n">
-        <v>1452.940444019866</v>
-      </c>
-      <c r="I648" t="n">
-        <v>462.3984642937558</v>
-      </c>
-      <c r="K648" t="n">
-        <v>-968.1964488346466</v>
-      </c>
-      <c r="M648" t="n">
-        <v>988.7677928593348</v>
-      </c>
-      <c r="O648" t="n">
-        <v>398.9740001975406</v>
-      </c>
-      <c r="Q648" t="n">
-        <v>1466.627743667644</v>
-      </c>
-      <c r="S648" t="n">
-        <v>1531.429508773223</v>
-      </c>
-    </row>
-    <row r="649">
-      <c r="A649" t="n">
-        <v>1065.812279048963</v>
-      </c>
-      <c r="C649" t="n">
-        <v>620.2498212238688</v>
-      </c>
-      <c r="E649" t="n">
-        <v>1692.218834031889</v>
-      </c>
-      <c r="G649" t="n">
-        <v>1453.339418020064</v>
-      </c>
-      <c r="I649" t="n">
-        <v>463.1204331444678</v>
-      </c>
-      <c r="K649" t="n">
-        <v>-968.0890338614745</v>
-      </c>
-      <c r="M649" t="n">
-        <v>988.7691949954842</v>
-      </c>
-      <c r="O649" t="n">
-        <v>399.5589086532618</v>
-      </c>
-      <c r="Q649" t="n">
-        <v>1467.33393738968</v>
-      </c>
-      <c r="S649" t="n">
-        <v>1532.136684853231</v>
-      </c>
-    </row>
-    <row r="650">
-      <c r="A650" t="n">
-        <v>1066.275399482107</v>
-      </c>
-      <c r="C650" t="n">
-        <v>619.2817321900073</v>
-      </c>
-      <c r="E650" t="n">
-        <v>1693.207603226885</v>
-      </c>
-      <c r="G650" t="n">
-        <v>1453.738976928717</v>
-      </c>
-      <c r="I650" t="n">
-        <v>463.8412945878372</v>
-      </c>
-      <c r="K650" t="n">
-        <v>-967.9809923603671</v>
-      </c>
-      <c r="M650" t="n">
-        <v>988.7703856859389</v>
-      </c>
-      <c r="O650" t="n">
-        <v>400.1433792846001</v>
-      </c>
-      <c r="Q650" t="n">
-        <v>1468.040115296954</v>
-      </c>
-      <c r="S650" t="n">
-        <v>1532.843876167844</v>
-      </c>
-    </row>
-    <row r="651">
-      <c r="A651" t="n">
-        <v>1066.739240776695</v>
-      </c>
-      <c r="C651" t="n">
-        <v>618.313751197647</v>
-      </c>
-      <c r="E651" t="n">
-        <v>1694.196373612571</v>
-      </c>
-      <c r="G651" t="n">
-        <v>1454.139120308002</v>
-      </c>
-      <c r="I651" t="n">
-        <v>464.5610450611457</v>
-      </c>
-      <c r="K651" t="n">
-        <v>-967.8723162415963</v>
-      </c>
-      <c r="M651" t="n">
-        <v>988.7713581754269</v>
-      </c>
-      <c r="O651" t="n">
-        <v>400.7274121252067</v>
-      </c>
-      <c r="Q651" t="n">
-        <v>1468.74627703556</v>
-      </c>
-      <c r="S651" t="n">
-        <v>1533.551083063926</v>
-      </c>
-    </row>
-    <row r="652">
-      <c r="A652" t="n">
-        <v>1067.203801821756</v>
-      </c>
-      <c r="C652" t="n">
-        <v>617.3458788814054</v>
-      </c>
-      <c r="E652" t="n">
-        <v>1695.185144970746</v>
-      </c>
-      <c r="G652" t="n">
-        <v>1454.539847720127</v>
-      </c>
-      <c r="I652" t="n">
-        <v>465.2796808409221</v>
-      </c>
-      <c r="K652" t="n">
-        <v>-967.7629971329225</v>
-      </c>
-      <c r="M652" t="n">
-        <v>988.7721053494261</v>
-      </c>
-      <c r="O652" t="n">
-        <v>401.3110071969095</v>
-      </c>
-      <c r="Q652" t="n">
-        <v>1469.45242223914</v>
-      </c>
-      <c r="S652" t="n">
-        <v>1534.258305900602</v>
-      </c>
-    </row>
-    <row r="653">
-      <c r="A653" t="n">
-        <v>1067.669081502597</v>
-      </c>
-      <c r="C653" t="n">
-        <v>616.3781158842725</v>
-      </c>
-      <c r="E653" t="n">
-        <v>1696.173917076095</v>
-      </c>
-      <c r="G653" t="n">
-        <v>1454.941158727324</v>
-      </c>
-      <c r="I653" t="n">
-        <v>465.9971980270257</v>
-      </c>
-      <c r="K653" t="n">
-        <v>-967.6530263579934</v>
-      </c>
-      <c r="M653" t="n">
-        <v>988.7726197052871</v>
-      </c>
-      <c r="O653" t="n">
-        <v>401.894164512214</v>
-      </c>
-      <c r="Q653" t="n">
-        <v>1470.158550528239</v>
-      </c>
-      <c r="S653" t="n">
-        <v>1534.965545049901</v>
-      </c>
-    </row>
-    <row r="654">
-      <c r="A654" t="n">
-        <v>1068.135078700624</v>
-      </c>
-      <c r="C654" t="n">
-        <v>615.4104628579145</v>
-      </c>
-      <c r="E654" t="n">
-        <v>1697.162689695801</v>
-      </c>
-      <c r="G654" t="n">
-        <v>1455.343052891836</v>
-      </c>
-      <c r="I654" t="n">
-        <v>466.7135925340062</v>
-      </c>
-      <c r="K654" t="n">
-        <v>-967.5423949208835</v>
-      </c>
-      <c r="M654" t="n">
-        <v>988.772893326086</v>
-      </c>
-      <c r="O654" t="n">
-        <v>402.4768840693014</v>
-      </c>
-      <c r="Q654" t="n">
-        <v>1470.864661509596</v>
-      </c>
-      <c r="S654" t="n">
-        <v>1535.672800897441</v>
-      </c>
-    </row>
-    <row r="655">
-      <c r="A655" t="n">
-        <v>1068.601792293158</v>
-      </c>
-      <c r="C655" t="n">
-        <v>614.4429204629936</v>
-      </c>
-      <c r="E655" t="n">
-        <v>1698.151462589127</v>
-      </c>
-      <c r="G655" t="n">
-        <v>1455.745529775905</v>
-      </c>
-      <c r="I655" t="n">
-        <v>467.4288600767795</v>
-      </c>
-      <c r="K655" t="n">
-        <v>-967.4310934805135</v>
-      </c>
-      <c r="M655" t="n">
-        <v>988.7729178476548</v>
-      </c>
-      <c r="O655" t="n">
-        <v>403.0591658506637</v>
-      </c>
-      <c r="Q655" t="n">
-        <v>1471.570754775394</v>
-      </c>
-      <c r="S655" t="n">
-        <v>1536.380073843179</v>
-      </c>
-    </row>
-    <row r="656">
-      <c r="A656" t="n">
-        <v>1069.069221153235</v>
-      </c>
-      <c r="C656" t="n">
-        <v>613.4754893695131</v>
-      </c>
-      <c r="E656" t="n">
-        <v>1699.140235506974</v>
-      </c>
-      <c r="G656" t="n">
-        <v>1456.148588941756</v>
-      </c>
-      <c r="I656" t="n">
-        <v>468.1429961567574</v>
-      </c>
-      <c r="K656" t="n">
-        <v>-967.3191123272318</v>
-      </c>
-      <c r="M656" t="n">
-        <v>988.7726844276585</v>
-      </c>
-      <c r="O656" t="n">
-        <v>403.6410098224223</v>
-      </c>
-      <c r="Q656" t="n">
-        <v>1472.276829902453</v>
-      </c>
-      <c r="S656" t="n">
-        <v>1537.087364302198</v>
-      </c>
-    </row>
-    <row r="657">
-      <c r="A657" t="n">
-        <v>1069.537364149392</v>
-      </c>
-      <c r="C657" t="n">
-        <v>612.5081702571858</v>
-      </c>
-      <c r="E657" t="n">
-        <v>1700.129008191402</v>
-      </c>
-      <c r="G657" t="n">
-        <v>1456.552229951579</v>
-      </c>
-      <c r="I657" t="n">
-        <v>468.8559960447947</v>
-      </c>
-      <c r="K657" t="n">
-        <v>-967.2064413593944</v>
-      </c>
-      <c r="M657" t="n">
-        <v>988.7721837071695</v>
-      </c>
-      <c r="O657" t="n">
-        <v>404.2224159293255</v>
-      </c>
-      <c r="Q657" t="n">
-        <v>1472.982886451359</v>
-      </c>
-      <c r="S657" t="n">
-        <v>1537.794672705567</v>
-      </c>
-    </row>
-    <row r="658">
-      <c r="A658" t="n">
-        <v>1070.006220145437</v>
-      </c>
-      <c r="C658" t="n">
-        <v>611.5409638158264</v>
-      </c>
-      <c r="E658" t="n">
-        <v>1701.117780375109</v>
-      </c>
-      <c r="G658" t="n">
-        <v>1456.956452367508</v>
-      </c>
-      <c r="I658" t="n">
-        <v>469.5678547682292</v>
-      </c>
-      <c r="K658" t="n">
-        <v>-967.0930700522149</v>
-      </c>
-      <c r="M658" t="n">
-        <v>988.7714057690573</v>
-      </c>
-      <c r="O658" t="n">
-        <v>404.8033840920198</v>
-      </c>
-      <c r="Q658" t="n">
-        <v>1473.688923965533</v>
-      </c>
-      <c r="S658" t="n">
-        <v>1538.501999501261</v>
-      </c>
-    </row>
-    <row r="659">
-      <c r="A659" t="n">
-        <v>1070.475788000205</v>
-      </c>
-      <c r="C659" t="n">
-        <v>610.5738707457742</v>
-      </c>
-      <c r="E659" t="n">
-        <v>1702.106551780878</v>
-      </c>
-      <c r="G659" t="n">
-        <v>1457.3612557516</v>
-      </c>
-      <c r="I659" t="n">
-        <v>470.2785670879166</v>
-      </c>
-      <c r="K659" t="n">
-        <v>-966.9789874275239</v>
-      </c>
-      <c r="M659" t="n">
-        <v>988.7703400979717</v>
-      </c>
-      <c r="O659" t="n">
-        <v>405.3839142052311</v>
-      </c>
-      <c r="Q659" t="n">
-        <v>1474.394941970217</v>
-      </c>
-      <c r="S659" t="n">
-        <v>1539.209345155153</v>
-      </c>
-    </row>
-    <row r="660">
-      <c r="A660" t="n">
-        <v>1070.946066567293</v>
-      </c>
-      <c r="C660" t="n">
-        <v>609.6068917583467</v>
-      </c>
-      <c r="E660" t="n">
-        <v>1703.095322120976</v>
-      </c>
-      <c r="G660" t="n">
-        <v>1457.766639665805</v>
-      </c>
-      <c r="I660" t="n">
-        <v>470.9881274800409</v>
-      </c>
-      <c r="K660" t="n">
-        <v>-966.8641820193216</v>
-      </c>
-      <c r="M660" t="n">
-        <v>988.7689755228166</v>
-      </c>
-      <c r="O660" t="n">
-        <v>405.9640061320806</v>
-      </c>
-      <c r="Q660" t="n">
-        <v>1475.100939971391</v>
-      </c>
-      <c r="S660" t="n">
-        <v>1539.916710152081</v>
-      </c>
-    </row>
-    <row r="661">
-      <c r="A661" t="n">
-        <v>1071.417054694773</v>
-      </c>
-      <c r="C661" t="n">
-        <v>608.6400275763274</v>
-      </c>
-      <c r="E661" t="n">
-        <v>1704.084091096499</v>
-      </c>
-      <c r="G661" t="n">
-        <v>1458.172603671937</v>
-      </c>
-      <c r="I661" t="n">
-        <v>471.6965301147411</v>
-      </c>
-      <c r="K661" t="n">
-        <v>-966.7486418353519</v>
-      </c>
-      <c r="M661" t="n">
-        <v>988.7673001730946</v>
-      </c>
-      <c r="O661" t="n">
-        <v>406.5436597015832</v>
-      </c>
-      <c r="Q661" t="n">
-        <v>1475.806917454595</v>
-      </c>
-      <c r="S661" t="n">
-        <v>1540.624094997014</v>
-      </c>
-    </row>
-    <row r="662">
-      <c r="A662" t="n">
-        <v>1071.888751224888</v>
-      </c>
-      <c r="C662" t="n">
-        <v>607.673278934492</v>
-      </c>
-      <c r="E662" t="n">
-        <v>1705.072858396672</v>
-      </c>
-      <c r="G662" t="n">
-        <v>1458.579147331639</v>
-      </c>
-      <c r="I662" t="n">
-        <v>472.4037688301905</v>
-      </c>
-      <c r="K662" t="n">
-        <v>-966.6323543165163</v>
-      </c>
-      <c r="M662" t="n">
-        <v>988.7653014120588</v>
-      </c>
-      <c r="O662" t="n">
-        <v>407.1228747027362</v>
-      </c>
-      <c r="Q662" t="n">
-        <v>1476.512873883655</v>
-      </c>
-      <c r="S662" t="n">
-        <v>1541.3315002163</v>
-      </c>
-    </row>
-    <row r="663">
-      <c r="A663" t="n">
-        <v>1072.361154993718</v>
-      </c>
-      <c r="C663" t="n">
-        <v>606.7066465801755</v>
-      </c>
-      <c r="E663" t="n">
-        <v>1706.061623698084</v>
-      </c>
-      <c r="G663" t="n">
-        <v>1458.986270206341</v>
-      </c>
-      <c r="I663" t="n">
-        <v>473.1098371062217</v>
-      </c>
-      <c r="K663" t="n">
-        <v>-966.5153062892387</v>
-      </c>
-      <c r="M663" t="n">
-        <v>988.7629657705475</v>
-      </c>
-      <c r="O663" t="n">
-        <v>407.7016508763336</v>
-      </c>
-      <c r="Q663" t="n">
-        <v>1477.218808699305</v>
-      </c>
-      <c r="S663" t="n">
-        <v>1542.03892635902</v>
-      </c>
-    </row>
-    <row r="664">
-      <c r="A664" t="n">
-        <v>1072.834264830824</v>
-      </c>
-      <c r="C664" t="n">
-        <v>605.7401312738863</v>
-      </c>
-      <c r="E664" t="n">
-        <v>1707.050386663855</v>
-      </c>
-      <c r="G664" t="n">
-        <v>1459.393971857218</v>
-      </c>
-      <c r="I664" t="n">
-        <v>473.8147280331759</v>
-      </c>
-      <c r="K664" t="n">
-        <v>-966.397483914534</v>
-      </c>
-      <c r="M664" t="n">
-        <v>988.7602788767254</v>
-      </c>
-      <c r="O664" t="n">
-        <v>408.2799879156482</v>
-      </c>
-      <c r="Q664" t="n">
-        <v>1477.924721317681</v>
-      </c>
-      <c r="S664" t="n">
-        <v>1542.746373998479</v>
-      </c>
-    </row>
-    <row r="665">
-      <c r="A665" t="n">
-        <v>1073.308079558857</v>
-      </c>
-      <c r="C665" t="n">
-        <v>604.7737337899717</v>
-      </c>
-      <c r="E665" t="n">
-        <v>1708.039146942732</v>
-      </c>
-      <c r="G665" t="n">
-        <v>1459.802251845133</v>
-      </c>
-      <c r="I665" t="n">
-        <v>474.5184342837092</v>
-      </c>
-      <c r="K665" t="n">
-        <v>-966.2788726316194</v>
-      </c>
-      <c r="M665" t="n">
-        <v>988.7572253726375</v>
-      </c>
-      <c r="O665" t="n">
-        <v>408.8578854521074</v>
-      </c>
-      <c r="Q665" t="n">
-        <v>1478.630611128692</v>
-      </c>
-      <c r="S665" t="n">
-        <v>1543.453843733798</v>
-      </c>
-    </row>
-    <row r="666">
-      <c r="A666" t="n">
-        <v>1073.782597993141</v>
-      </c>
-      <c r="C666" t="n">
-        <v>603.8074549173401</v>
-      </c>
-      <c r="E666" t="n">
-        <v>1709.027904168104</v>
-      </c>
-      <c r="G666" t="n">
-        <v>1460.211109730586</v>
-      </c>
-      <c r="I666" t="n">
-        <v>475.2209480668625</v>
-      </c>
-      <c r="K666" t="n">
-        <v>-966.1594570932266</v>
-      </c>
-      <c r="M666" t="n">
-        <v>988.7537888207589</v>
-      </c>
-      <c r="O666" t="n">
-        <v>409.4353430507454</v>
-      </c>
-      <c r="Q666" t="n">
-        <v>1479.336477494239</v>
-      </c>
-      <c r="S666" t="n">
-        <v>1544.161336191675</v>
-      </c>
-    </row>
-    <row r="667">
-      <c r="A667" t="n">
-        <v>1074.257818941208</v>
-      </c>
-      <c r="C667" t="n">
-        <v>602.8412954602469</v>
-      </c>
-      <c r="E667" t="n">
-        <v>1710.016657956925</v>
-      </c>
-      <c r="G667" t="n">
-        <v>1460.620545073636</v>
-      </c>
-      <c r="I667" t="n">
-        <v>475.9222610998677</v>
-      </c>
-      <c r="K667" t="n">
-        <v>-966.0392210969349</v>
-      </c>
-      <c r="M667" t="n">
-        <v>988.749951603495</v>
-      </c>
-      <c r="O667" t="n">
-        <v>410.0123601997439</v>
-      </c>
-      <c r="Q667" t="n">
-        <v>1480.042319746274</v>
-      </c>
-      <c r="S667" t="n">
-        <v>1544.868852028289</v>
-      </c>
-    </row>
-    <row r="668">
-      <c r="A668" t="n">
-        <v>1074.733741202308</v>
-      </c>
-      <c r="C668" t="n">
-        <v>601.87525623915</v>
-      </c>
-      <c r="E668" t="n">
-        <v>1711.005407908528</v>
-      </c>
-      <c r="G668" t="n">
-        <v>1461.030557433836</v>
-      </c>
-      <c r="I668" t="n">
-        <v>476.6223645508489</v>
-      </c>
-      <c r="K668" t="n">
-        <v>-965.9181475030891</v>
-      </c>
-      <c r="M668" t="n">
-        <v>988.7456948106319</v>
-      </c>
-      <c r="O668" t="n">
-        <v>410.588936302247</v>
-      </c>
-      <c r="Q668" t="n">
-        <v>1480.748137184668</v>
-      </c>
-      <c r="S668" t="n">
-        <v>1545.576391931404</v>
-      </c>
-    </row>
-    <row r="669">
-      <c r="A669" t="n">
-        <v>1075.210363566858</v>
-      </c>
-      <c r="C669" t="n">
-        <v>600.9093380916469</v>
-      </c>
-      <c r="E669" t="n">
-        <v>1711.994153603339</v>
-      </c>
-      <c r="G669" t="n">
-        <v>1461.441146370138</v>
-      </c>
-      <c r="I669" t="n">
-        <v>477.3212489965317</v>
-      </c>
-      <c r="K669" t="n">
-        <v>-965.796218147716</v>
-      </c>
-      <c r="M669" t="n">
-        <v>988.7409981045039</v>
-      </c>
-      <c r="O669" t="n">
-        <v>411.1650706602177</v>
-      </c>
-      <c r="Q669" t="n">
-        <v>1481.453929074879</v>
-      </c>
-      <c r="S669" t="n">
-        <v>1546.283956622655</v>
-      </c>
-    </row>
-    <row r="670">
-      <c r="A670" t="n">
-        <v>1075.687684815855</v>
-      </c>
-      <c r="C670" t="n">
-        <v>599.9435418734992</v>
-      </c>
-      <c r="E670" t="n">
-        <v>1712.982894601444</v>
-      </c>
-      <c r="G670" t="n">
-        <v>1461.852311440799</v>
-      </c>
-      <c r="I670" t="n">
-        <v>478.0189043599421</v>
-      </c>
-      <c r="K670" t="n">
-        <v>-965.673413741797</v>
-      </c>
-      <c r="M670" t="n">
-        <v>988.7358395803858</v>
-      </c>
-      <c r="O670" t="n">
-        <v>411.7407624632961</v>
-      </c>
-      <c r="Q670" t="n">
-        <v>1482.159694645388</v>
-      </c>
-      <c r="S670" t="n">
-        <v>1546.991546860076</v>
-      </c>
-    </row>
-    <row r="671">
-      <c r="A671" t="n">
-        <v>1076.165703720215</v>
-      </c>
-      <c r="C671" t="n">
-        <v>598.9778684597574</v>
-      </c>
-      <c r="E671" t="n">
-        <v>1713.971630441024</v>
-      </c>
-      <c r="G671" t="n">
-        <v>1462.264052203262</v>
-      </c>
-      <c r="I671" t="n">
-        <v>478.7153198519718</v>
-      </c>
-      <c r="K671" t="n">
-        <v>-965.5497137579232</v>
-      </c>
-      <c r="M671" t="n">
-        <v>988.730195600283</v>
-      </c>
-      <c r="O671" t="n">
-        <v>412.3160107737931</v>
-      </c>
-      <c r="Q671" t="n">
-        <v>1482.865433084876</v>
-      </c>
-      <c r="S671" t="n">
-        <v>1547.699163440875</v>
-      </c>
-    </row>
-    <row r="672">
-      <c r="A672" t="n">
-        <v>1076.644419040067</v>
-      </c>
-      <c r="C672" t="n">
-        <v>598.0123187459994</v>
-      </c>
-      <c r="E672" t="n">
-        <v>1714.960360636624</v>
-      </c>
-      <c r="G672" t="n">
-        <v>1462.676368214036</v>
-      </c>
-      <c r="I672" t="n">
-        <v>479.4104838911153</v>
-      </c>
-      <c r="K672" t="n">
-        <v>-965.4250963035338</v>
-      </c>
-      <c r="M672" t="n">
-        <v>988.7240406039837</v>
-      </c>
-      <c r="O672" t="n">
-        <v>412.8908145039532</v>
-      </c>
-      <c r="Q672" t="n">
-        <v>1483.5711435391</v>
-      </c>
-      <c r="S672" t="n">
-        <v>1548.406807204504</v>
-      </c>
-    </row>
-    <row r="673">
-      <c r="A673" t="n">
-        <v>1077.123829523958</v>
-      </c>
-      <c r="C673" t="n">
-        <v>597.0468936496959</v>
-      </c>
-      <c r="E673" t="n">
-        <v>1715.949084677228</v>
-      </c>
-      <c r="G673" t="n">
-        <v>1463.08925902854</v>
-      </c>
-      <c r="I673" t="n">
-        <v>480.1043840316197</v>
-      </c>
-      <c r="K673" t="n">
-        <v>-965.2995379734648</v>
-      </c>
-      <c r="M673" t="n">
-        <v>988.7173469012396</v>
-      </c>
-      <c r="O673" t="n">
-        <v>413.4651724007199</v>
-      </c>
-      <c r="Q673" t="n">
-        <v>1484.276825107449</v>
-      </c>
-      <c r="S673" t="n">
-        <v>1549.114479036053</v>
-      </c>
-    </row>
-    <row r="674">
-      <c r="A674" t="n">
-        <v>1077.60393390799</v>
-      </c>
-      <c r="C674" t="n">
-        <v>596.0815941117224</v>
-      </c>
-      <c r="E674" t="n">
-        <v>1716.937802024129</v>
-      </c>
-      <c r="G674" t="n">
-        <v>1463.50272420094</v>
-      </c>
-      <c r="I674" t="n">
-        <v>480.7970068634404</v>
-      </c>
-      <c r="K674" t="n">
-        <v>-965.1730136855576</v>
-      </c>
-      <c r="M674" t="n">
-        <v>988.7100844268844</v>
-      </c>
-      <c r="O674" t="n">
-        <v>414.0390830123124</v>
-      </c>
-      <c r="Q674" t="n">
-        <v>1484.982476839099</v>
-      </c>
-      <c r="S674" t="n">
-        <v>1549.822179870022</v>
-      </c>
-    </row>
-    <row r="675">
-      <c r="A675" t="n">
-        <v>1078.084730914853</v>
-      </c>
-      <c r="C675" t="n">
-        <v>595.1164210980369</v>
-      </c>
-      <c r="E675" t="n">
-        <v>1717.926512108556</v>
-      </c>
-      <c r="G675" t="n">
-        <v>1463.916763283953</v>
-      </c>
-      <c r="I675" t="n">
-        <v>481.4883379096955</v>
-      </c>
-      <c r="K675" t="n">
-        <v>-965.0454964913706</v>
-      </c>
-      <c r="M675" t="n">
-        <v>988.7022204638924</v>
-      </c>
-      <c r="O675" t="n">
-        <v>414.61254467049</v>
-      </c>
-      <c r="Q675" t="n">
-        <v>1485.688097728761</v>
-      </c>
-      <c r="S675" t="n">
-        <v>1550.529910694506</v>
-      </c>
-    </row>
-    <row r="676">
-      <c r="A676" t="n">
-        <v>1078.566219252763</v>
-      </c>
-      <c r="C676" t="n">
-        <v>594.1513756015455</v>
-      </c>
-      <c r="E676" t="n">
-        <v>1718.91521432902</v>
-      </c>
-      <c r="G676" t="n">
-        <v>1464.331375828623</v>
-      </c>
-      <c r="I676" t="n">
-        <v>482.1783615057029</v>
-      </c>
-      <c r="K676" t="n">
-        <v>-964.9169573585823</v>
-      </c>
-      <c r="M676" t="n">
-        <v>988.6937193252834</v>
-      </c>
-      <c r="O676" t="n">
-        <v>415.1855554448503</v>
-      </c>
-      <c r="Q676" t="n">
-        <v>1486.393686711911</v>
-      </c>
-      <c r="S676" t="n">
-        <v>1551.237672555887</v>
-      </c>
-    </row>
-    <row r="677">
-      <c r="A677" t="n">
-        <v>1079.048397614268</v>
-      </c>
-      <c r="C677" t="n">
-        <v>593.1864586441869</v>
-      </c>
-      <c r="E677" t="n">
-        <v>1719.903908048346</v>
-      </c>
-      <c r="G677" t="n">
-        <v>1464.746561384068</v>
-      </c>
-      <c r="I677" t="n">
-        <v>482.8670606609649</v>
-      </c>
-      <c r="K677" t="n">
-        <v>-964.7873649180383</v>
-      </c>
-      <c r="M677" t="n">
-        <v>988.6845419853216</v>
-      </c>
-      <c r="O677" t="n">
-        <v>415.7581131132702</v>
-      </c>
-      <c r="Q677" t="n">
-        <v>1487.099242659465</v>
-      </c>
-      <c r="S677" t="n">
-        <v>1551.945466564063</v>
-      </c>
-    </row>
-    <row r="678">
-      <c r="A678" t="n">
-        <v>1079.531264674929</v>
-      </c>
-      <c r="C678" t="n">
-        <v>592.2216712792689</v>
-      </c>
-      <c r="E678" t="n">
-        <v>1720.892592590331</v>
-      </c>
-      <c r="G678" t="n">
-        <v>1465.162319497181</v>
-      </c>
-      <c r="I678" t="n">
-        <v>483.5544168981869</v>
-      </c>
-      <c r="K678" t="n">
-        <v>-964.6566851756688</v>
-      </c>
-      <c r="M678" t="n">
-        <v>988.6746456522815</v>
-      </c>
-      <c r="O678" t="n">
-        <v>416.3302151087009</v>
-      </c>
-      <c r="Q678" t="n">
-        <v>1487.804764371785</v>
-      </c>
-      <c r="S678" t="n">
-        <v>1552.653293898347</v>
-      </c>
-    </row>
-    <row r="679">
-      <c r="A679" t="n">
-        <v>1080.014819091828</v>
-      </c>
-      <c r="C679" t="n">
-        <v>591.2570145940932</v>
-      </c>
-      <c r="E679" t="n">
-        <v>1721.881267235983</v>
-      </c>
-      <c r="G679" t="n">
-        <v>1465.57864971229</v>
-      </c>
-      <c r="I679" t="n">
-        <v>484.2404100691056</v>
-      </c>
-      <c r="K679" t="n">
-        <v>-964.5248811747251</v>
-      </c>
-      <c r="M679" t="n">
-        <v>988.663983272545</v>
-      </c>
-      <c r="O679" t="n">
-        <v>416.9018584652804</v>
-      </c>
-      <c r="Q679" t="n">
-        <v>1488.510250571935</v>
-      </c>
-      <c r="S679" t="n">
-        <v>1553.361155814089</v>
-      </c>
-    </row>
-    <row r="680">
-      <c r="A680" t="n">
-        <v>1080.499059501897</v>
-      </c>
-      <c r="C680" t="n">
-        <v>590.2924897129185</v>
-      </c>
-      <c r="E680" t="n">
-        <v>1722.869931219256</v>
-      </c>
-      <c r="G680" t="n">
-        <v>1465.995551570755</v>
-      </c>
-      <c r="I680" t="n">
-        <v>484.9250181393927</v>
-      </c>
-      <c r="K680" t="n">
-        <v>-964.3919125990124</v>
-      </c>
-      <c r="M680" t="n">
-        <v>988.652502945115</v>
-      </c>
-      <c r="O680" t="n">
-        <v>417.473039753304</v>
-      </c>
-      <c r="Q680" t="n">
-        <v>1489.215699898034</v>
-      </c>
-      <c r="S680" t="n">
-        <v>1554.069053650195</v>
-      </c>
-    </row>
-    <row r="681">
-      <c r="A681" t="n">
-        <v>1080.983984520036</v>
-      </c>
-      <c r="C681" t="n">
-        <v>589.3280978003195</v>
-      </c>
-      <c r="E681" t="n">
-        <v>1723.858583722201</v>
-      </c>
-      <c r="G681" t="n">
-        <v>1466.413024610509</v>
-      </c>
-      <c r="I681" t="n">
-        <v>485.608216935816</v>
-      </c>
-      <c r="K681" t="n">
-        <v>-964.2577353104116</v>
-      </c>
-      <c r="M681" t="n">
-        <v>988.64014724154</v>
-      </c>
-      <c r="O681" t="n">
-        <v>418.0437550005536</v>
-      </c>
-      <c r="Q681" t="n">
-        <v>1489.92111089459</v>
-      </c>
-      <c r="S681" t="n">
-        <v>1554.776988837639</v>
-      </c>
-    </row>
-    <row r="682">
-      <c r="A682" t="n">
-        <v>1081.469592736972</v>
-      </c>
-      <c r="C682" t="n">
-        <v>588.3638400650091</v>
-      </c>
-      <c r="E682" t="n">
-        <v>1724.847223869442</v>
-      </c>
-      <c r="G682" t="n">
-        <v>1466.831068365509</v>
-      </c>
-      <c r="I682" t="n">
-        <v>486.2899798536091</v>
-      </c>
-      <c r="K682" t="n">
-        <v>-964.1223008019324</v>
-      </c>
-      <c r="M682" t="n">
-        <v>988.6268523939634</v>
-      </c>
-      <c r="O682" t="n">
-        <v>418.6139995981648</v>
-      </c>
-      <c r="Q682" t="n">
-        <v>1490.626482002595</v>
-      </c>
-      <c r="S682" t="n">
-        <v>1555.4849629092</v>
-      </c>
-    </row>
-    <row r="683">
-      <c r="A683" t="n">
-        <v>1081.955882716825</v>
-      </c>
-      <c r="C683" t="n">
-        <v>587.3997177642071</v>
-      </c>
-      <c r="E683" t="n">
-        <v>1725.835850721836</v>
-      </c>
-      <c r="G683" t="n">
-        <v>1467.249682365107</v>
-      </c>
-      <c r="I683" t="n">
-        <v>486.9702775010865</v>
-      </c>
-      <c r="K683" t="n">
-        <v>-963.9855555478789</v>
-      </c>
-      <c r="M683" t="n">
-        <v>988.6125473299217</v>
-      </c>
-      <c r="O683" t="n">
-        <v>419.1837681830748</v>
-      </c>
-      <c r="Q683" t="n">
-        <v>1491.331811548187</v>
-      </c>
-      <c r="S683" t="n">
-        <v>1556.192977510596</v>
-      </c>
-    </row>
-    <row r="684">
-      <c r="A684" t="n">
-        <v>1082.442852994327</v>
-      </c>
-      <c r="C684" t="n">
-        <v>586.4357322086593</v>
-      </c>
-      <c r="E684" t="n">
-        <v>1726.824463269166</v>
-      </c>
-      <c r="G684" t="n">
-        <v>1467.66886613329</v>
-      </c>
-      <c r="I684" t="n">
-        <v>487.6490772874149</v>
-      </c>
-      <c r="K684" t="n">
-        <v>-963.8474402244128</v>
-      </c>
-      <c r="M684" t="n">
-        <v>988.5971525245623</v>
-      </c>
-      <c r="O684" t="n">
-        <v>419.7530545054633</v>
-      </c>
-      <c r="Q684" t="n">
-        <v>1492.037097729599</v>
-      </c>
-      <c r="S684" t="n">
-        <v>1556.901034413309</v>
-      </c>
-    </row>
-    <row r="685">
-      <c r="A685" t="n">
-        <v>1082.930502071614</v>
-      </c>
-      <c r="C685" t="n">
-        <v>585.4718847684348</v>
-      </c>
-      <c r="E685" t="n">
-        <v>1727.813060421691</v>
-      </c>
-      <c r="G685" t="n">
-        <v>1468.088619187796</v>
-      </c>
-      <c r="I685" t="n">
-        <v>488.3263429242106</v>
-      </c>
-      <c r="K685" t="n">
-        <v>-963.7078887762982</v>
-      </c>
-      <c r="M685" t="n">
-        <v>988.5805786068431</v>
-      </c>
-      <c r="O685" t="n">
-        <v>420.3218512527656</v>
-      </c>
-      <c r="Q685" t="n">
-        <v>1492.742338602046</v>
-      </c>
-      <c r="S685" t="n">
-        <v>1557.609135529422</v>
-      </c>
-    </row>
-    <row r="686">
-      <c r="A686" t="n">
-        <v>1083.418828414538</v>
-      </c>
-      <c r="C686" t="n">
-        <v>584.5081768796585</v>
-      </c>
-      <c r="E686" t="n">
-        <v>1728.801641000298</v>
-      </c>
-      <c r="G686" t="n">
-        <v>1468.508941039049</v>
-      </c>
-      <c r="I686" t="n">
-        <v>489.0020338189061</v>
-      </c>
-      <c r="K686" t="n">
-        <v>-963.5668272841258</v>
-      </c>
-      <c r="M686" t="n">
-        <v>988.5627246778768</v>
-      </c>
-      <c r="O686" t="n">
-        <v>420.890149847537</v>
-      </c>
-      <c r="Q686" t="n">
-        <v>1493.447532060154</v>
-      </c>
-      <c r="S686" t="n">
-        <v>1558.31728292888</v>
-      </c>
-    </row>
-    <row r="687">
-      <c r="A687" t="n">
-        <v>1083.907830448357</v>
-      </c>
-      <c r="C687" t="n">
-        <v>583.5446100523744</v>
-      </c>
-      <c r="E687" t="n">
-        <v>1729.790203724976</v>
-      </c>
-      <c r="G687" t="n">
-        <v>1468.929831188896</v>
-      </c>
-      <c r="I687" t="n">
-        <v>489.6761043478364</v>
-      </c>
-      <c r="K687" t="n">
-        <v>-963.4241725791526</v>
-      </c>
-      <c r="M687" t="n">
-        <v>988.5434762445584</v>
-      </c>
-      <c r="O687" t="n">
-        <v>421.4579401823357</v>
-      </c>
-      <c r="Q687" t="n">
-        <v>1494.152675817374</v>
-      </c>
-      <c r="S687" t="n">
-        <v>1559.0254788597</v>
-      </c>
-    </row>
-    <row r="688">
-      <c r="A688" t="n">
-        <v>1084.397506552705</v>
-      </c>
-      <c r="C688" t="n">
-        <v>582.5811858797953</v>
-      </c>
-      <c r="E688" t="n">
-        <v>1730.77874720122</v>
-      </c>
-      <c r="G688" t="n">
-        <v>1469.351289129078</v>
-      </c>
-      <c r="I688" t="n">
-        <v>490.3485029574313</v>
-      </c>
-      <c r="K688" t="n">
-        <v>-963.2798305398182</v>
-      </c>
-      <c r="M688" t="n">
-        <v>988.5227026809389</v>
-      </c>
-      <c r="O688" t="n">
-        <v>422.0252103000348</v>
-      </c>
-      <c r="Q688" t="n">
-        <v>1494.857767381749</v>
-      </c>
-      <c r="S688" t="n">
-        <v>1559.733725771765</v>
-      </c>
-    </row>
-    <row r="689">
-      <c r="A689" t="n">
-        <v>1084.887855055662</v>
-      </c>
-      <c r="C689" t="n">
-        <v>581.6179060492555</v>
-      </c>
-      <c r="E689" t="n">
-        <v>1731.767269903901</v>
-      </c>
-      <c r="G689" t="n">
-        <v>1469.773314339378</v>
-      </c>
-      <c r="Q689" t="n">
-        <v>1495.562804027148</v>
-      </c>
-      <c r="S689" t="n">
-        <v>1560.442026345058</v>
       </c>
     </row>
   </sheetData>

</xml_diff>